<commit_message>
Trying out submodules for shared files in Server and Client
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b5af9c88eeda555/Documents/GitHub/Twosion/FusionCards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50785AF3-9C73-478A-B25A-BE7C09D45164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{50785AF3-9C73-478A-B25A-BE7C09D45164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7A268AF-6324-4D15-A8DE-33FA925E53AE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{33AB78CB-5412-47F2-92BF-14E232D6F736}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>name</t>
   </si>
@@ -62,18 +62,9 @@
     <t>WATER</t>
   </si>
   <si>
-    <t>BEAST</t>
-  </si>
-  <si>
-    <t>NECRO</t>
-  </si>
-  <si>
     <t>ROCK</t>
   </si>
   <si>
-    <t>MECH</t>
-  </si>
-  <si>
     <t>_null_art.png</t>
   </si>
   <si>
@@ -83,16 +74,28 @@
     <t>_water_art.png</t>
   </si>
   <si>
-    <t>_bease_art.png</t>
-  </si>
-  <si>
-    <t>_necro_art.png</t>
-  </si>
-  <si>
     <t>_rock_art.png</t>
   </si>
   <si>
-    <t>_mech_art.png</t>
+    <t>elements</t>
+  </si>
+  <si>
+    <t>NATURE</t>
+  </si>
+  <si>
+    <t>_nature_art.png</t>
+  </si>
+  <si>
+    <t>DEATH</t>
+  </si>
+  <si>
+    <t>TECH</t>
+  </si>
+  <si>
+    <t>_tech_art.png</t>
+  </si>
+  <si>
+    <t>_death_art.png</t>
   </si>
 </sst>
 </file>
@@ -448,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F97F9BB-1D6F-48B2-8A9B-3CA0B4335FC0}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,9 +463,10 @@
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="46.85546875" customWidth="1"/>
+    <col min="6" max="6" width="63.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -476,15 +480,18 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -492,13 +499,16 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -506,13 +516,16 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -520,52 +533,64 @@
       <c r="D4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>4</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="C6">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>17</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -575,6 +600,9 @@
       </c>
       <c r="D8">
         <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>